<commit_message>
Excel File Read Changes
</commit_message>
<xml_diff>
--- a/src/main/resources/static/users.xlsx
+++ b/src/main/resources/static/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aj629\IdeaProjects\GEET_API\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20A2CDE-0029-4810-9878-BB7302E07B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C195520D-65A5-4515-A26E-6332996BC41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="271">
   <si>
     <t>Id</t>
   </si>
@@ -1105,8 +1105,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="C93" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5882,7 +5882,9 @@
       <c r="E100" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F100" s="1"/>
+      <c r="F100" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="G100" s="1">
         <v>656820</v>
       </c>

</xml_diff>